<commit_message>
Update Verilog Stopwatch Requirments.xlsx
</commit_message>
<xml_diff>
--- a/Verilog Stopwatch Requirments.xlsx
+++ b/Verilog Stopwatch Requirments.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010371\Documents\VHDL Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Documents\GitHub\Verilog_Stopwatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84224FAB-1016-4CD7-8A92-CB1E6AC9DF71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC685BCF-BFC3-4149-89E2-1E4F73CC0899}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection" sheetId="1" r:id="rId1"/>
     <sheet name="10ms Timer" sheetId="2" r:id="rId2"/>
     <sheet name="20-Bit Counter" sheetId="3" r:id="rId3"/>
-    <sheet name="7-Seg Decoder" sheetId="4" r:id="rId4"/>
+    <sheet name="20-bit BCD to 7-Segment Display" sheetId="4" r:id="rId4"/>
     <sheet name="General" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -71,16 +71,94 @@
   </si>
   <si>
     <t>Initialization</t>
+  </si>
+  <si>
+    <t>20-bit BCD to 7-Segment Display Driver</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout1 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout2 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout3 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout4 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout5 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout1 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout2 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout3 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout4 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout5 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>DRV</t>
+  </si>
+  <si>
+    <t>DRV_INIT_01</t>
+  </si>
+  <si>
+    <t>DRV_INIT_02</t>
+  </si>
+  <si>
+    <t>DRV_INIT_03</t>
+  </si>
+  <si>
+    <t>DRV_INIT_04</t>
+  </si>
+  <si>
+    <t>DRV_INIT_05</t>
+  </si>
+  <si>
+    <t>DRV_INIT_06</t>
+  </si>
+  <si>
+    <t>DRV_INIT_07</t>
+  </si>
+  <si>
+    <t>DRV_INIT_08</t>
+  </si>
+  <si>
+    <t>DRV_INIT_09</t>
+  </si>
+  <si>
+    <t>DRV_INIT_10</t>
+  </si>
+  <si>
+    <t>DRV_MAP_01</t>
+  </si>
+  <si>
+    <t>BCD to 7-segment mapping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -102,11 +180,98 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -116,6 +281,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,20 +626,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B4EAFD-D6BC-4B33-AEA7-1FB008F58338}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -463,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -480,7 +673,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -503,7 +696,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -515,7 +708,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -523,12 +716,152 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B94154-4E96-428E-BDF1-A1ABE2650270}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="8"/>
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="8"/>
+      <c r="D5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="D8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="D9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="8"/>
+      <c r="D10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="12"/>
+      <c r="D11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:C11"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -539,7 +872,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -725,6 +1058,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -733,20 +1072,38 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
+    <ds:schemaRef ds:uri="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>